<commit_message>
updating seabird data prep
Removed Aie sandbar, adjusted calculations of adult/nesting seabirds based on Jayna's responses. Added "side of motu" as another scale.
</commit_message>
<xml_diff>
--- a/seabird_data/raw_data/seabird_transects_to_use.xlsx
+++ b/seabird_data/raw_data/seabird_transects_to_use.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Benkwitt/Documents/GitHub/TARP_motu_comparison/seabird_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Benkwitt/Documents/GitHub/TARP_motu_comparison/seabird_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA10E423-1B70-4742-9325-6B8206C3DF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B90FB6-0AD2-B94D-9C33-E8695200A1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29120" yWindow="-2200" windowWidth="31100" windowHeight="15740" xr2:uid="{A7104C0C-CF60-2F41-B53F-E73003247C94}"/>
+    <workbookView xWindow="-35980" yWindow="-2840" windowWidth="35600" windowHeight="16220" xr2:uid="{A7104C0C-CF60-2F41-B53F-E73003247C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>Motu</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Side</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>Aie</t>
   </si>
   <si>
@@ -189,6 +186,45 @@
   </si>
   <si>
     <t>Transect name (alternative name) - Closest 100 m</t>
+  </si>
+  <si>
+    <t>notes_100-200m_transects</t>
+  </si>
+  <si>
+    <t>notes_side_of_motu</t>
+  </si>
+  <si>
+    <t>Transect Sequence - Side of Motu</t>
+  </si>
+  <si>
+    <t>0945-0946-0947-0948</t>
+  </si>
+  <si>
+    <t>0948-0949-0950-0945</t>
+  </si>
+  <si>
+    <t>1143-1144-1145-1146-1147-1148-1149-1150-1151-1152</t>
+  </si>
+  <si>
+    <t>0837-0838-0839-1137-1138-1139-1140-1141-1142-1143</t>
+  </si>
+  <si>
+    <t>obvious split to e/w corners of motu, just added 1 extra transect to 200 m</t>
+  </si>
+  <si>
+    <t>obvious split to n/s corners of motu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only included until eastern most corner (so excluded northern stretch which is cut-off from transects). Obvious southern corner. </t>
+  </si>
+  <si>
+    <t>only included until northwestern corner (so excluded norther stretch which is cut-off from transects). Obvious southern corner</t>
+  </si>
+  <si>
+    <t>0631 - 0632 - 0633 - 0634 - 0635 - 0636 - 0637 - 0638 - 0644 - 0645 - 0646 - 0647 - 0648 - 0686 - 0687 - 0688 - 0689 - 0690 - 0691  - 0692</t>
+  </si>
+  <si>
+    <t>0692 - 0693 - 0694 - 0695 - 0696 - 0697 - 0698 - 0699 - 0700 - 0701 - 0702 - 0606</t>
   </si>
 </sst>
 </file>
@@ -561,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BC5F6D-8E4C-0A4B-BAC8-ED71E0504A6B}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -574,12 +610,14 @@
     <col min="4" max="4" width="19.1640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="28.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="49.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="49.1640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -587,199 +625,241 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="G2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="5" t="s">
+    <row r="4" spans="1:11" ht="136" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="D6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>21</v>
+      <c r="K7" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>